<commit_message>
Update Paytm parser formatting, mapping rules, and README
</commit_message>
<xml_diff>
--- a/Reference Documents/Merchant category mapping.xlsx
+++ b/Reference Documents/Merchant category mapping.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\PN1PEPF000069CE\EXCELCNV\49e9f7f0-0e47-4a29-91cd-d22b829fc26f\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="8_{2EE984B8-BE7D-42A6-B46C-4DDEACA32909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22734B9A-1215-4228-90A1-CFAA01B11B5D}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="8_{2EE984B8-BE7D-42A6-B46C-4DDEACA32909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9E8B021-1AB8-4EF8-AFBD-6B40B212293B}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" firstSheet="1" activeTab="2" xr2:uid="{C92CC430-4B32-4796-8D62-416574D6DE36}"/>
   </bookViews>
   <sheets>
     <sheet name="Merchant category mapping" sheetId="1" r:id="rId1"/>
-    <sheet name="PayTm" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="PayTm_0" sheetId="2" r:id="rId2"/>
+    <sheet name="PayTm_1" sheetId="4" r:id="rId3"/>
     <sheet name="UPI Name" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="217">
   <si>
     <t>Keyword Pattern</t>
   </si>
@@ -663,6 +663,15 @@
   </si>
   <si>
     <t>Airtel</t>
+  </si>
+  <si>
+    <t>#🪙 Investment</t>
+  </si>
+  <si>
+    <t>Gold Coin Redemption</t>
+  </si>
+  <si>
+    <t>PayTm Gold Coin</t>
   </si>
   <si>
     <t>File Name</t>
@@ -2917,8 +2926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC94042-E3C1-46A3-9AF7-530C61664ADD}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14:K33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3364,10 +3373,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91AF2A8D-08DB-402A-B65E-BCCAEF7E03A5}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D20"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3376,9 +3385,12 @@
     <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>151</v>
       </c>
@@ -3391,8 +3403,14 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="15" t="s">
         <v>175</v>
       </c>
@@ -3405,8 +3423,14 @@
       <c r="D2" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="15" t="s">
         <v>175</v>
       </c>
@@ -3417,8 +3441,14 @@
       <c r="D3" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="F3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="15" t="s">
         <v>179</v>
       </c>
@@ -3431,8 +3461,14 @@
       <c r="D4" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="16" t="s">
         <v>181</v>
       </c>
@@ -3446,7 +3482,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>181</v>
       </c>
@@ -3460,7 +3496,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7" s="15" t="s">
         <v>187</v>
       </c>
@@ -3472,7 +3508,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8" s="15" t="s">
         <v>189</v>
       </c>
@@ -3484,7 +3520,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9" s="15" t="s">
         <v>191</v>
       </c>
@@ -3496,7 +3532,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10" s="15" t="s">
         <v>192</v>
       </c>
@@ -3510,7 +3546,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11" s="15" t="s">
         <v>192</v>
       </c>
@@ -3520,7 +3556,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12" s="15" t="s">
         <v>197</v>
       </c>
@@ -3532,7 +3568,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13" s="15" t="s">
         <v>198</v>
       </c>
@@ -3546,7 +3582,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:7">
       <c r="A14" s="15" t="s">
         <v>198</v>
       </c>
@@ -3560,7 +3596,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7">
       <c r="A15" s="15" t="s">
         <v>200</v>
       </c>
@@ -3574,7 +3610,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16" s="15" t="s">
         <v>201</v>
       </c>
@@ -3592,7 +3628,7 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>202</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>12</v>
@@ -3630,6 +3666,20 @@
       </c>
       <c r="D20" s="1" t="s">
         <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="B21" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" t="s">
+        <v>172</v>
+      </c>
+      <c r="D21" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3652,42 +3702,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>